<commit_message>
[fix][asset] Fix column bug to download asset
</commit_message>
<xml_diff>
--- a/api/template/server_template.xlsx
+++ b/api/template/server_template.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>机柜</t>
   </si>
@@ -99,10 +99,10 @@
     <t>内存</t>
   </si>
   <si>
-    <t>硬盘</t>
-  </si>
-  <si>
-    <t>RAID</t>
+    <t>系统盘</t>
+  </si>
+  <si>
+    <t>数据盘</t>
   </si>
   <si>
     <t>网卡</t>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>IB卡</t>
+  </si>
+  <si>
+    <t>模块</t>
+  </si>
+  <si>
+    <t>配件变更</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1098,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2462,23 +2468,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="20.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="20.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="20.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.625" style="1" customWidth="1"/>
+    <col min="4" max="11" width="20.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:9">
+    <row r="1" ht="15.75" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -2505,6 +2508,12 @@
       </c>
       <c r="I1" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>